<commit_message>
Update Complaint Closure Database.xlsx
</commit_message>
<xml_diff>
--- a/Complaint Closure Database.xlsx
+++ b/Complaint Closure Database.xlsx
@@ -19,7 +19,7 @@
     <definedName name="_2G_Cell_Id">Lists!$G$2:$G$7241</definedName>
     <definedName name="_3G_Cell_ID">Lists!$H$2:$H$10953</definedName>
     <definedName name="_4G_Cell_ID">Lists!$I$2:$I$2801</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RF_CC_Database!$A$1:$BD$242</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RF_CC_Database!$A$1:$BC$242</definedName>
     <definedName name="_Technology">Lists!$N$2:$N$8</definedName>
     <definedName name="Call_Quality">Lists!$F$2:$F$4</definedName>
     <definedName name="City">Lists!$B$2:$B$1019</definedName>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="1761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="1763">
   <si>
     <t>Sr No.</t>
   </si>
@@ -5331,6 +5331,12 @@
   </si>
   <si>
     <t>Comments Closure</t>
+  </si>
+  <si>
+    <t>Issue Resolved as per customer</t>
+  </si>
+  <si>
+    <t>Other region complaint</t>
   </si>
 </sst>
 </file>
@@ -5384,7 +5390,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5427,6 +5433,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5441,7 +5453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="69"/>
@@ -5484,6 +5496,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment textRotation="69"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="69"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5766,11 +5781,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD242"/>
+  <dimension ref="A1:BC242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5786,10 +5801,10 @@
     <col min="35" max="35" width="7.1796875" customWidth="1"/>
     <col min="40" max="40" width="15.7265625" customWidth="1"/>
     <col min="41" max="41" width="9.90625" customWidth="1"/>
-    <col min="54" max="54" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="116.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:55" ht="116.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5907,10 +5922,10 @@
       <c r="AM1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="19" t="s">
         <v>38</v>
       </c>
       <c r="AP1" s="1" t="s">
@@ -5938,1017 +5953,1014 @@
         <v>31</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AY1" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="AY1" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="AZ1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="BA1" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="BA1" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="BB1" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="BC1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB2" s="8"/>
-      <c r="BC2" s="13"/>
-    </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB3" s="8"/>
-      <c r="BC3" s="13"/>
-    </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="13"/>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA3" s="8"/>
+      <c r="BB3" s="13"/>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.35">
       <c r="AB4" s="12"/>
-      <c r="BB4" s="8"/>
-      <c r="BC4" s="13"/>
-    </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB5" s="8"/>
-      <c r="BC5" s="13"/>
-    </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="BA4" s="8"/>
+      <c r="BB4" s="13"/>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA5" s="8"/>
+      <c r="BB5" s="13"/>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.35">
       <c r="AB6" s="10"/>
-      <c r="BB6" s="8"/>
-      <c r="BC6" s="13"/>
-    </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB7" s="8"/>
-      <c r="BC7" s="13"/>
-    </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB8" s="8"/>
-      <c r="BC8" s="13"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB9" s="8"/>
-      <c r="BC9" s="13"/>
-    </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB10" s="8"/>
-      <c r="BC10" s="13"/>
-    </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB11" s="8"/>
-      <c r="BC11" s="13"/>
-    </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB12" s="8"/>
-      <c r="BC12" s="13"/>
-    </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB13" s="8"/>
-      <c r="BC13" s="13"/>
-    </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB14" s="8"/>
-      <c r="BC14" s="13"/>
-    </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB15" s="8"/>
-      <c r="BC15" s="13"/>
-    </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="BB16" s="8"/>
-      <c r="BC16" s="13"/>
-    </row>
-    <row r="17" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA6" s="8"/>
+      <c r="BB6" s="13"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA7" s="8"/>
+      <c r="BB7" s="13"/>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA8" s="8"/>
+      <c r="BB8" s="13"/>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA9" s="8"/>
+      <c r="BB9" s="13"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA10" s="8"/>
+      <c r="BB10" s="13"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA11" s="8"/>
+      <c r="BB11" s="13"/>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA12" s="8"/>
+      <c r="BB12" s="13"/>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA13" s="8"/>
+      <c r="BB13" s="13"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA14" s="8"/>
+      <c r="BB14" s="13"/>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA15" s="8"/>
+      <c r="BB15" s="13"/>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="BA16" s="8"/>
+      <c r="BB16" s="13"/>
+    </row>
+    <row r="17" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB17" s="12"/>
-      <c r="BB17" s="8"/>
-      <c r="BC17" s="13"/>
-    </row>
-    <row r="18" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB18" s="8"/>
-      <c r="BC18" s="13"/>
-    </row>
-    <row r="19" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB19" s="8"/>
-      <c r="BC19" s="13"/>
-    </row>
-    <row r="20" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA17" s="8"/>
+      <c r="BB17" s="13"/>
+    </row>
+    <row r="18" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA18" s="8"/>
+      <c r="BB18" s="13"/>
+    </row>
+    <row r="19" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA19" s="8"/>
+      <c r="BB19" s="13"/>
+    </row>
+    <row r="20" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB20" s="12"/>
-      <c r="BB20" s="8"/>
-      <c r="BC20" s="13"/>
-    </row>
-    <row r="21" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB21" s="8"/>
-      <c r="BC21" s="13"/>
-    </row>
-    <row r="22" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA20" s="8"/>
+      <c r="BB20" s="13"/>
+    </row>
+    <row r="21" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA21" s="8"/>
+      <c r="BB21" s="13"/>
+    </row>
+    <row r="22" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB22" s="11"/>
-      <c r="BB22" s="8"/>
-      <c r="BC22" s="13"/>
-    </row>
-    <row r="23" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB23" s="8"/>
-      <c r="BC23" s="13"/>
-    </row>
-    <row r="24" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB24" s="8"/>
-      <c r="BC24" s="13"/>
-    </row>
-    <row r="25" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB25" s="8"/>
-      <c r="BC25" s="13"/>
-    </row>
-    <row r="26" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB26" s="8"/>
-      <c r="BC26" s="13"/>
-    </row>
-    <row r="27" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB27" s="8"/>
-      <c r="BC27" s="13"/>
-    </row>
-    <row r="28" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB28" s="8"/>
-      <c r="BC28" s="13"/>
-    </row>
-    <row r="29" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB29" s="8"/>
-    </row>
-    <row r="30" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB30" s="8"/>
-      <c r="BC30" s="13"/>
-    </row>
-    <row r="31" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB31" s="8"/>
-      <c r="BC31" s="13"/>
-    </row>
-    <row r="32" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB32" s="8"/>
-      <c r="BC32" s="13"/>
-    </row>
-    <row r="33" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB33" s="8"/>
-      <c r="BC33" s="13"/>
-    </row>
-    <row r="34" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB34" s="8"/>
-      <c r="BC34" s="13"/>
-    </row>
-    <row r="35" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB35" s="8"/>
-      <c r="BC35" s="13"/>
-    </row>
-    <row r="36" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB36" s="8"/>
-      <c r="BC36" s="13"/>
-    </row>
-    <row r="37" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB37" s="8"/>
-      <c r="BC37" s="13"/>
-    </row>
-    <row r="38" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB38" s="8"/>
-      <c r="BC38" s="13"/>
-    </row>
-    <row r="39" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB39" s="8"/>
-      <c r="BC39" s="13"/>
-    </row>
-    <row r="40" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB40" s="8"/>
-      <c r="BC40" s="13"/>
-    </row>
-    <row r="41" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB41" s="8"/>
-      <c r="BC41" s="13"/>
-    </row>
-    <row r="42" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB42" s="8"/>
-      <c r="BC42" s="13"/>
-    </row>
-    <row r="43" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB43" s="8"/>
-      <c r="BC43" s="13"/>
-    </row>
-    <row r="44" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB44" s="8"/>
-      <c r="BC44" s="13"/>
-    </row>
-    <row r="45" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB45" s="8"/>
-      <c r="BC45" s="13"/>
-    </row>
-    <row r="46" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB46" s="8"/>
-      <c r="BC46" s="13"/>
-    </row>
-    <row r="47" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA22" s="8"/>
+      <c r="BB22" s="13"/>
+    </row>
+    <row r="23" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA23" s="8"/>
+      <c r="BB23" s="13"/>
+    </row>
+    <row r="24" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA24" s="8"/>
+      <c r="BB24" s="13"/>
+    </row>
+    <row r="25" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA25" s="8"/>
+      <c r="BB25" s="13"/>
+    </row>
+    <row r="26" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA26" s="8"/>
+      <c r="BB26" s="13"/>
+    </row>
+    <row r="27" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA27" s="8"/>
+      <c r="BB27" s="13"/>
+    </row>
+    <row r="28" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA28" s="8"/>
+      <c r="BB28" s="13"/>
+    </row>
+    <row r="29" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA29" s="8"/>
+    </row>
+    <row r="30" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA30" s="8"/>
+      <c r="BB30" s="13"/>
+    </row>
+    <row r="31" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA31" s="8"/>
+      <c r="BB31" s="13"/>
+    </row>
+    <row r="32" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA32" s="8"/>
+      <c r="BB32" s="13"/>
+    </row>
+    <row r="33" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA33" s="8"/>
+      <c r="BB33" s="13"/>
+    </row>
+    <row r="34" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA34" s="8"/>
+      <c r="BB34" s="13"/>
+    </row>
+    <row r="35" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA35" s="8"/>
+      <c r="BB35" s="13"/>
+    </row>
+    <row r="36" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA36" s="8"/>
+      <c r="BB36" s="13"/>
+    </row>
+    <row r="37" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA37" s="8"/>
+      <c r="BB37" s="13"/>
+    </row>
+    <row r="38" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA38" s="8"/>
+      <c r="BB38" s="13"/>
+    </row>
+    <row r="39" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA39" s="8"/>
+      <c r="BB39" s="13"/>
+    </row>
+    <row r="40" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA40" s="8"/>
+      <c r="BB40" s="13"/>
+    </row>
+    <row r="41" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA41" s="8"/>
+      <c r="BB41" s="13"/>
+    </row>
+    <row r="42" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA42" s="8"/>
+      <c r="BB42" s="13"/>
+    </row>
+    <row r="43" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA43" s="8"/>
+      <c r="BB43" s="13"/>
+    </row>
+    <row r="44" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA44" s="8"/>
+      <c r="BB44" s="13"/>
+    </row>
+    <row r="45" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA45" s="8"/>
+      <c r="BB45" s="13"/>
+    </row>
+    <row r="46" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA46" s="8"/>
+      <c r="BB46" s="13"/>
+    </row>
+    <row r="47" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB47" s="12"/>
-      <c r="BB47" s="8"/>
-      <c r="BC47" s="13"/>
-    </row>
-    <row r="48" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA47" s="8"/>
+      <c r="BB47" s="13"/>
+    </row>
+    <row r="48" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB48" s="12"/>
-      <c r="BB48" s="8"/>
-      <c r="BC48" s="13"/>
-    </row>
-    <row r="49" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB49" s="8"/>
-      <c r="BC49" s="13"/>
-    </row>
-    <row r="50" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB50" s="8"/>
-      <c r="BC50" s="13"/>
-    </row>
-    <row r="51" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB51" s="8"/>
-      <c r="BC51" s="13"/>
-    </row>
-    <row r="52" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB52" s="8"/>
-      <c r="BC52" s="13"/>
-    </row>
-    <row r="53" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB53" s="8"/>
-      <c r="BC53" s="13"/>
-    </row>
-    <row r="54" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB54" s="8"/>
-      <c r="BC54" s="13"/>
-    </row>
-    <row r="55" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB55" s="8"/>
-      <c r="BC55" s="13"/>
-    </row>
-    <row r="56" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB56" s="8"/>
-      <c r="BC56" s="13"/>
-    </row>
-    <row r="57" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB57" s="8"/>
-      <c r="BC57" s="13"/>
-    </row>
-    <row r="58" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB58" s="8"/>
-      <c r="BC58" s="13"/>
-    </row>
-    <row r="59" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB59" s="8"/>
-      <c r="BC59" s="13"/>
-    </row>
-    <row r="60" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB60" s="8"/>
-      <c r="BC60" s="13"/>
-    </row>
-    <row r="61" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB61" s="8"/>
-      <c r="BC61" s="13"/>
-    </row>
-    <row r="62" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB62" s="8"/>
-      <c r="BC62" s="13"/>
-    </row>
-    <row r="63" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB63" s="8"/>
-      <c r="BC63" s="13"/>
-    </row>
-    <row r="64" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB64" s="8"/>
-      <c r="BC64" s="13"/>
-    </row>
-    <row r="65" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB65" s="8"/>
-      <c r="BC65" s="13"/>
-    </row>
-    <row r="66" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB66" s="8"/>
-      <c r="BC66" s="13"/>
-    </row>
-    <row r="68" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA48" s="8"/>
+      <c r="BB48" s="13"/>
+    </row>
+    <row r="49" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA49" s="8"/>
+      <c r="BB49" s="13"/>
+    </row>
+    <row r="50" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA50" s="8"/>
+      <c r="BB50" s="13"/>
+    </row>
+    <row r="51" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA51" s="8"/>
+      <c r="BB51" s="13"/>
+    </row>
+    <row r="52" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA52" s="8"/>
+      <c r="BB52" s="13"/>
+    </row>
+    <row r="53" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA53" s="8"/>
+      <c r="BB53" s="13"/>
+    </row>
+    <row r="54" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA54" s="8"/>
+      <c r="BB54" s="13"/>
+    </row>
+    <row r="55" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA55" s="8"/>
+      <c r="BB55" s="13"/>
+    </row>
+    <row r="56" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA56" s="8"/>
+      <c r="BB56" s="13"/>
+    </row>
+    <row r="57" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA57" s="8"/>
+      <c r="BB57" s="13"/>
+    </row>
+    <row r="58" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA58" s="8"/>
+      <c r="BB58" s="13"/>
+    </row>
+    <row r="59" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA59" s="8"/>
+      <c r="BB59" s="13"/>
+    </row>
+    <row r="60" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA60" s="8"/>
+      <c r="BB60" s="13"/>
+    </row>
+    <row r="61" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA61" s="8"/>
+      <c r="BB61" s="13"/>
+    </row>
+    <row r="62" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA62" s="8"/>
+      <c r="BB62" s="13"/>
+    </row>
+    <row r="63" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA63" s="8"/>
+      <c r="BB63" s="13"/>
+    </row>
+    <row r="64" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA64" s="8"/>
+      <c r="BB64" s="13"/>
+    </row>
+    <row r="65" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA65" s="8"/>
+      <c r="BB65" s="13"/>
+    </row>
+    <row r="66" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA66" s="8"/>
+      <c r="BB66" s="13"/>
+    </row>
+    <row r="68" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB68" s="12"/>
-      <c r="BB68" s="8"/>
-      <c r="BC68" s="13"/>
-    </row>
-    <row r="69" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB69" s="8"/>
-      <c r="BC69" s="13"/>
-    </row>
-    <row r="70" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB70" s="8"/>
-      <c r="BC70" s="13"/>
-    </row>
-    <row r="71" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB71" s="8"/>
-      <c r="BC71" s="13"/>
-    </row>
-    <row r="72" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB72" s="8"/>
-      <c r="BC72" s="13"/>
-    </row>
-    <row r="73" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB73" s="8"/>
-      <c r="BC73" s="13"/>
-    </row>
-    <row r="74" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB74" s="8"/>
-      <c r="BC74" s="13"/>
-    </row>
-    <row r="75" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB75" s="8"/>
-      <c r="BC75" s="13"/>
-    </row>
-    <row r="76" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB76" s="8"/>
-      <c r="BC76" s="13"/>
-    </row>
-    <row r="77" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB77" s="8"/>
-      <c r="BC77" s="13"/>
-    </row>
-    <row r="78" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB78" s="8"/>
-      <c r="BC78" s="13"/>
-    </row>
-    <row r="79" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB79" s="8"/>
-      <c r="BC79" s="13"/>
-    </row>
-    <row r="80" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB80" s="8"/>
-      <c r="BC80" s="13"/>
-    </row>
-    <row r="81" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB81" s="8"/>
-      <c r="BC81" s="13"/>
-    </row>
-    <row r="82" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB82" s="8"/>
-      <c r="BC82" s="13"/>
-    </row>
-    <row r="83" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB83" s="8"/>
-      <c r="BC83" s="13"/>
-    </row>
-    <row r="84" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB84" s="8"/>
-      <c r="BC84" s="13"/>
-    </row>
-    <row r="85" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB85" s="8"/>
-      <c r="BC85" s="13"/>
-    </row>
-    <row r="86" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB86" s="8"/>
-      <c r="BC86" s="13"/>
-    </row>
-    <row r="87" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB87" s="8"/>
-      <c r="BC87" s="13"/>
-    </row>
-    <row r="88" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB88" s="8"/>
-      <c r="BC88" s="13"/>
-    </row>
-    <row r="89" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB89" s="8"/>
-      <c r="BC89" s="13"/>
-    </row>
-    <row r="90" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB90" s="8"/>
-      <c r="BC90" s="13"/>
-    </row>
-    <row r="91" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB91" s="8"/>
-      <c r="BC91" s="13"/>
-    </row>
-    <row r="92" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB92" s="8"/>
-      <c r="BC92" s="13"/>
-    </row>
-    <row r="93" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB93" s="8"/>
-      <c r="BC93" s="13"/>
-    </row>
-    <row r="94" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB94" s="8"/>
-      <c r="BC94" s="13"/>
-    </row>
-    <row r="95" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB95" s="8"/>
-      <c r="BC95" s="13"/>
-    </row>
-    <row r="96" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB96" s="8"/>
-      <c r="BC96" s="13"/>
-    </row>
-    <row r="97" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB97" s="8"/>
-      <c r="BC97" s="13"/>
-    </row>
-    <row r="98" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB98" s="8"/>
-      <c r="BC98" s="13"/>
-    </row>
-    <row r="99" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB99" s="8"/>
-      <c r="BC99" s="13"/>
-    </row>
-    <row r="100" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB100" s="8"/>
-      <c r="BC100" s="13"/>
-    </row>
-    <row r="101" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB101" s="8"/>
-      <c r="BC101" s="13"/>
-    </row>
-    <row r="102" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB102" s="8"/>
-      <c r="BC102" s="13"/>
-    </row>
-    <row r="103" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB103" s="8"/>
-      <c r="BC103" s="13"/>
-    </row>
-    <row r="104" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB104" s="8"/>
-      <c r="BC104" s="13"/>
-    </row>
-    <row r="105" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB105" s="8"/>
-      <c r="BC105" s="13"/>
-    </row>
-    <row r="106" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB106" s="8"/>
-      <c r="BC106" s="13"/>
-    </row>
-    <row r="107" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB107" s="8"/>
-      <c r="BC107" s="13"/>
-    </row>
-    <row r="108" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB108" s="8"/>
-      <c r="BC108" s="13"/>
-    </row>
-    <row r="109" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB109" s="8"/>
-      <c r="BC109" s="13"/>
-    </row>
-    <row r="110" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB110" s="8"/>
-      <c r="BC110" s="13"/>
-    </row>
-    <row r="111" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB111" s="8"/>
-      <c r="BC111" s="13"/>
-    </row>
-    <row r="112" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB112" s="8"/>
-      <c r="BC112" s="13"/>
-    </row>
-    <row r="113" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB113" s="8"/>
-      <c r="BC113" s="13"/>
-    </row>
-    <row r="114" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB114" s="8"/>
-      <c r="BC114" s="13"/>
-    </row>
-    <row r="115" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB115" s="8"/>
-      <c r="BC115" s="13"/>
-    </row>
-    <row r="116" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB116" s="8"/>
-      <c r="BC116" s="13"/>
-    </row>
-    <row r="117" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB117" s="8"/>
-      <c r="BC117" s="13"/>
-    </row>
-    <row r="118" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB118" s="8"/>
-      <c r="BC118" s="13"/>
-    </row>
-    <row r="119" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB119" s="8"/>
-      <c r="BC119" s="13"/>
-    </row>
-    <row r="120" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB120" s="8"/>
-      <c r="BC120" s="13"/>
-    </row>
-    <row r="121" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB121" s="8"/>
-      <c r="BC121" s="13"/>
-    </row>
-    <row r="122" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB122" s="8"/>
-      <c r="BC122" s="13"/>
-    </row>
-    <row r="123" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB123" s="8"/>
-      <c r="BC123" s="13"/>
-    </row>
-    <row r="124" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB124" s="8"/>
-      <c r="BC124" s="13"/>
-    </row>
-    <row r="125" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA68" s="8"/>
+      <c r="BB68" s="13"/>
+    </row>
+    <row r="69" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA69" s="8"/>
+      <c r="BB69" s="13"/>
+    </row>
+    <row r="70" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA70" s="8"/>
+      <c r="BB70" s="13"/>
+    </row>
+    <row r="71" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA71" s="8"/>
+      <c r="BB71" s="13"/>
+    </row>
+    <row r="72" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA72" s="8"/>
+      <c r="BB72" s="13"/>
+    </row>
+    <row r="73" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA73" s="8"/>
+      <c r="BB73" s="13"/>
+    </row>
+    <row r="74" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA74" s="8"/>
+      <c r="BB74" s="13"/>
+    </row>
+    <row r="75" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA75" s="8"/>
+      <c r="BB75" s="13"/>
+    </row>
+    <row r="76" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA76" s="8"/>
+      <c r="BB76" s="13"/>
+    </row>
+    <row r="77" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA77" s="8"/>
+      <c r="BB77" s="13"/>
+    </row>
+    <row r="78" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA78" s="8"/>
+      <c r="BB78" s="13"/>
+    </row>
+    <row r="79" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA79" s="8"/>
+      <c r="BB79" s="13"/>
+    </row>
+    <row r="80" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA80" s="8"/>
+      <c r="BB80" s="13"/>
+    </row>
+    <row r="81" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA81" s="8"/>
+      <c r="BB81" s="13"/>
+    </row>
+    <row r="82" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA82" s="8"/>
+      <c r="BB82" s="13"/>
+    </row>
+    <row r="83" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA83" s="8"/>
+      <c r="BB83" s="13"/>
+    </row>
+    <row r="84" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA84" s="8"/>
+      <c r="BB84" s="13"/>
+    </row>
+    <row r="85" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA85" s="8"/>
+      <c r="BB85" s="13"/>
+    </row>
+    <row r="86" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA86" s="8"/>
+      <c r="BB86" s="13"/>
+    </row>
+    <row r="87" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA87" s="8"/>
+      <c r="BB87" s="13"/>
+    </row>
+    <row r="88" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA88" s="8"/>
+      <c r="BB88" s="13"/>
+    </row>
+    <row r="89" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA89" s="8"/>
+      <c r="BB89" s="13"/>
+    </row>
+    <row r="90" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA90" s="8"/>
+      <c r="BB90" s="13"/>
+    </row>
+    <row r="91" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA91" s="8"/>
+      <c r="BB91" s="13"/>
+    </row>
+    <row r="92" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA92" s="8"/>
+      <c r="BB92" s="13"/>
+    </row>
+    <row r="93" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA93" s="8"/>
+      <c r="BB93" s="13"/>
+    </row>
+    <row r="94" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA94" s="8"/>
+      <c r="BB94" s="13"/>
+    </row>
+    <row r="95" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA95" s="8"/>
+      <c r="BB95" s="13"/>
+    </row>
+    <row r="96" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA96" s="8"/>
+      <c r="BB96" s="13"/>
+    </row>
+    <row r="97" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA97" s="8"/>
+      <c r="BB97" s="13"/>
+    </row>
+    <row r="98" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA98" s="8"/>
+      <c r="BB98" s="13"/>
+    </row>
+    <row r="99" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA99" s="8"/>
+      <c r="BB99" s="13"/>
+    </row>
+    <row r="100" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA100" s="8"/>
+      <c r="BB100" s="13"/>
+    </row>
+    <row r="101" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA101" s="8"/>
+      <c r="BB101" s="13"/>
+    </row>
+    <row r="102" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA102" s="8"/>
+      <c r="BB102" s="13"/>
+    </row>
+    <row r="103" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA103" s="8"/>
+      <c r="BB103" s="13"/>
+    </row>
+    <row r="104" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA104" s="8"/>
+      <c r="BB104" s="13"/>
+    </row>
+    <row r="105" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA105" s="8"/>
+      <c r="BB105" s="13"/>
+    </row>
+    <row r="106" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA106" s="8"/>
+      <c r="BB106" s="13"/>
+    </row>
+    <row r="107" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA107" s="8"/>
+      <c r="BB107" s="13"/>
+    </row>
+    <row r="108" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA108" s="8"/>
+      <c r="BB108" s="13"/>
+    </row>
+    <row r="109" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA109" s="8"/>
+      <c r="BB109" s="13"/>
+    </row>
+    <row r="110" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA110" s="8"/>
+      <c r="BB110" s="13"/>
+    </row>
+    <row r="111" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA111" s="8"/>
+      <c r="BB111" s="13"/>
+    </row>
+    <row r="112" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA112" s="8"/>
+      <c r="BB112" s="13"/>
+    </row>
+    <row r="113" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA113" s="8"/>
+      <c r="BB113" s="13"/>
+    </row>
+    <row r="114" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA114" s="8"/>
+      <c r="BB114" s="13"/>
+    </row>
+    <row r="115" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA115" s="8"/>
+      <c r="BB115" s="13"/>
+    </row>
+    <row r="116" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA116" s="8"/>
+      <c r="BB116" s="13"/>
+    </row>
+    <row r="117" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA117" s="8"/>
+      <c r="BB117" s="13"/>
+    </row>
+    <row r="118" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA118" s="8"/>
+      <c r="BB118" s="13"/>
+    </row>
+    <row r="119" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA119" s="8"/>
+      <c r="BB119" s="13"/>
+    </row>
+    <row r="120" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA120" s="8"/>
+      <c r="BB120" s="13"/>
+    </row>
+    <row r="121" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA121" s="8"/>
+      <c r="BB121" s="13"/>
+    </row>
+    <row r="122" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA122" s="8"/>
+      <c r="BB122" s="13"/>
+    </row>
+    <row r="123" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA123" s="8"/>
+      <c r="BB123" s="13"/>
+    </row>
+    <row r="124" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA124" s="8"/>
+      <c r="BB124" s="13"/>
+    </row>
+    <row r="125" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB125" s="12"/>
-      <c r="BB125" s="8"/>
-      <c r="BC125" s="13"/>
-    </row>
-    <row r="126" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB126" s="8"/>
-      <c r="BC126" s="13"/>
-    </row>
-    <row r="127" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB127" s="8"/>
-      <c r="BC127" s="13"/>
-    </row>
-    <row r="128" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB128" s="8"/>
-      <c r="BC128" s="13"/>
-    </row>
-    <row r="129" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB129" s="8"/>
-      <c r="BC129" s="13"/>
-    </row>
-    <row r="130" spans="27:56" x14ac:dyDescent="0.35">
+      <c r="BA125" s="8"/>
+      <c r="BB125" s="13"/>
+    </row>
+    <row r="126" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA126" s="8"/>
+      <c r="BB126" s="13"/>
+    </row>
+    <row r="127" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA127" s="8"/>
+      <c r="BB127" s="13"/>
+    </row>
+    <row r="128" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA128" s="8"/>
+      <c r="BB128" s="13"/>
+    </row>
+    <row r="129" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA129" s="8"/>
+      <c r="BB129" s="13"/>
+    </row>
+    <row r="130" spans="27:55" x14ac:dyDescent="0.35">
       <c r="AB130" s="12"/>
-      <c r="BB130" s="8"/>
-      <c r="BC130" s="13"/>
-    </row>
-    <row r="131" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB131" s="8"/>
-      <c r="BC131" s="13"/>
-    </row>
-    <row r="132" spans="27:56" x14ac:dyDescent="0.35">
+      <c r="BA130" s="8"/>
+      <c r="BB130" s="13"/>
+    </row>
+    <row r="131" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA131" s="8"/>
+      <c r="BB131" s="13"/>
+    </row>
+    <row r="132" spans="27:55" x14ac:dyDescent="0.35">
       <c r="AB132" s="12"/>
-      <c r="BB132" s="8"/>
-      <c r="BC132" s="13"/>
-    </row>
-    <row r="133" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB133" s="8"/>
-      <c r="BC133" s="13"/>
-    </row>
-    <row r="134" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB134" s="8"/>
-      <c r="BC134" s="13"/>
-    </row>
-    <row r="135" spans="27:56" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="BA132" s="8"/>
+      <c r="BB132" s="13"/>
+    </row>
+    <row r="133" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA133" s="8"/>
+      <c r="BB133" s="13"/>
+    </row>
+    <row r="134" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA134" s="8"/>
+      <c r="BB134" s="13"/>
+    </row>
+    <row r="135" spans="27:55" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="AA135"/>
-      <c r="BB135" s="8"/>
-      <c r="BC135" s="13"/>
-      <c r="BD135"/>
-    </row>
-    <row r="136" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB136" s="8"/>
-      <c r="BC136" s="13"/>
-    </row>
-    <row r="137" spans="27:56" x14ac:dyDescent="0.35">
+      <c r="BA135" s="8"/>
+      <c r="BB135" s="13"/>
+      <c r="BC135"/>
+    </row>
+    <row r="136" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA136" s="8"/>
+      <c r="BB136" s="13"/>
+    </row>
+    <row r="137" spans="27:55" x14ac:dyDescent="0.35">
       <c r="AB137" s="12"/>
-      <c r="BB137" s="8"/>
-      <c r="BC137" s="13"/>
-    </row>
-    <row r="138" spans="27:56" x14ac:dyDescent="0.35">
+      <c r="BA137" s="8"/>
+      <c r="BB137" s="13"/>
+    </row>
+    <row r="138" spans="27:55" x14ac:dyDescent="0.35">
       <c r="AB138" s="12"/>
-      <c r="BB138" s="8"/>
-      <c r="BC138" s="13"/>
-    </row>
-    <row r="139" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB139" s="8"/>
-      <c r="BC139" s="13"/>
-    </row>
-    <row r="140" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB140" s="8"/>
-      <c r="BC140" s="13"/>
-    </row>
-    <row r="141" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB141" s="8"/>
-      <c r="BC141" s="13"/>
-    </row>
-    <row r="142" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB142" s="8"/>
-      <c r="BC142" s="13"/>
-    </row>
-    <row r="143" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB143" s="8"/>
-      <c r="BC143" s="13"/>
-    </row>
-    <row r="144" spans="27:56" x14ac:dyDescent="0.35">
-      <c r="BB144" s="8"/>
-      <c r="BC144" s="13"/>
-    </row>
-    <row r="145" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB145" s="8"/>
-      <c r="BC145" s="13"/>
-    </row>
-    <row r="146" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA138" s="8"/>
+      <c r="BB138" s="13"/>
+    </row>
+    <row r="139" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA139" s="8"/>
+      <c r="BB139" s="13"/>
+    </row>
+    <row r="140" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA140" s="8"/>
+      <c r="BB140" s="13"/>
+    </row>
+    <row r="141" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA141" s="8"/>
+      <c r="BB141" s="13"/>
+    </row>
+    <row r="142" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA142" s="8"/>
+      <c r="BB142" s="13"/>
+    </row>
+    <row r="143" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA143" s="8"/>
+      <c r="BB143" s="13"/>
+    </row>
+    <row r="144" spans="27:55" x14ac:dyDescent="0.35">
+      <c r="BA144" s="8"/>
+      <c r="BB144" s="13"/>
+    </row>
+    <row r="145" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA145" s="8"/>
+      <c r="BB145" s="13"/>
+    </row>
+    <row r="146" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB146" s="12"/>
-      <c r="BB146" s="8"/>
-      <c r="BC146" s="13"/>
-    </row>
-    <row r="147" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB147" s="8"/>
-      <c r="BC147" s="13"/>
-    </row>
-    <row r="148" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB148" s="8"/>
-      <c r="BC148" s="13"/>
-    </row>
-    <row r="149" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB149" s="8"/>
-      <c r="BC149" s="13"/>
-    </row>
-    <row r="150" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA146" s="8"/>
+      <c r="BB146" s="13"/>
+    </row>
+    <row r="147" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA147" s="8"/>
+      <c r="BB147" s="13"/>
+    </row>
+    <row r="148" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA148" s="8"/>
+      <c r="BB148" s="13"/>
+    </row>
+    <row r="149" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA149" s="8"/>
+      <c r="BB149" s="13"/>
+    </row>
+    <row r="150" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB150" s="15"/>
-      <c r="BB150" s="8"/>
-      <c r="BC150" s="13"/>
-    </row>
-    <row r="151" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA150" s="8"/>
+      <c r="BB150" s="13"/>
+    </row>
+    <row r="151" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB151" s="12"/>
-      <c r="BB151" s="8"/>
-      <c r="BC151" s="13"/>
-    </row>
-    <row r="152" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB152" s="8"/>
-      <c r="BC152" s="13"/>
-    </row>
-    <row r="153" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB153" s="8"/>
-      <c r="BC153" s="13"/>
-    </row>
-    <row r="154" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA151" s="8"/>
+      <c r="BB151" s="13"/>
+    </row>
+    <row r="152" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA152" s="8"/>
+      <c r="BB152" s="13"/>
+    </row>
+    <row r="153" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA153" s="8"/>
+      <c r="BB153" s="13"/>
+    </row>
+    <row r="154" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB154" s="12"/>
-      <c r="BB154" s="8"/>
-      <c r="BC154" s="13"/>
-    </row>
-    <row r="155" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA154" s="8"/>
+      <c r="BB154" s="13"/>
+    </row>
+    <row r="155" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB155" s="12"/>
-      <c r="BB155" s="8"/>
-      <c r="BC155" s="13"/>
-    </row>
-    <row r="156" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB156" s="8"/>
-      <c r="BC156" s="13"/>
-    </row>
-    <row r="157" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB157" s="8"/>
-      <c r="BC157" s="13"/>
-    </row>
-    <row r="158" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA155" s="8"/>
+      <c r="BB155" s="13"/>
+    </row>
+    <row r="156" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA156" s="8"/>
+      <c r="BB156" s="13"/>
+    </row>
+    <row r="157" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA157" s="8"/>
+      <c r="BB157" s="13"/>
+    </row>
+    <row r="158" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB158" s="12"/>
-      <c r="BB158" s="8"/>
-      <c r="BC158" s="13"/>
-    </row>
-    <row r="159" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB159" s="8"/>
-      <c r="BC159" s="13"/>
-    </row>
-    <row r="160" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB160" s="8"/>
-      <c r="BC160" s="13"/>
-    </row>
-    <row r="161" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA158" s="8"/>
+      <c r="BB158" s="13"/>
+    </row>
+    <row r="159" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA159" s="8"/>
+      <c r="BB159" s="13"/>
+    </row>
+    <row r="160" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA160" s="8"/>
+      <c r="BB160" s="13"/>
+    </row>
+    <row r="161" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB161" s="12"/>
-      <c r="BB161" s="8"/>
-      <c r="BC161" s="13"/>
-    </row>
-    <row r="162" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA161" s="8"/>
+      <c r="BB161" s="13"/>
+    </row>
+    <row r="162" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB162" s="12"/>
-      <c r="BB162" s="8"/>
-      <c r="BC162" s="13"/>
-    </row>
-    <row r="163" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB163" s="8"/>
-      <c r="BC163" s="13"/>
-    </row>
-    <row r="164" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB164" s="8"/>
-      <c r="BC164" s="13"/>
-    </row>
-    <row r="165" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB165" s="8"/>
-      <c r="BC165" s="13"/>
-    </row>
-    <row r="166" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB166" s="8"/>
-      <c r="BC166" s="13"/>
-    </row>
-    <row r="167" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB167" s="8"/>
-      <c r="BC167" s="13"/>
-    </row>
-    <row r="168" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA162" s="8"/>
+      <c r="BB162" s="13"/>
+    </row>
+    <row r="163" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA163" s="8"/>
+      <c r="BB163" s="13"/>
+    </row>
+    <row r="164" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA164" s="8"/>
+      <c r="BB164" s="13"/>
+    </row>
+    <row r="165" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA165" s="8"/>
+      <c r="BB165" s="13"/>
+    </row>
+    <row r="166" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA166" s="8"/>
+      <c r="BB166" s="13"/>
+    </row>
+    <row r="167" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA167" s="8"/>
+      <c r="BB167" s="13"/>
+    </row>
+    <row r="168" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB168" s="16"/>
-      <c r="BB168" s="8"/>
-      <c r="BC168" s="13"/>
-    </row>
-    <row r="169" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB169" s="8"/>
-      <c r="BC169" s="13"/>
-    </row>
-    <row r="170" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB170" s="8"/>
-      <c r="BC170" s="13"/>
-    </row>
-    <row r="171" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB171" s="8"/>
-      <c r="BC171" s="13"/>
-    </row>
-    <row r="172" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB172" s="8"/>
-      <c r="BC172" s="13"/>
-    </row>
-    <row r="173" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB173" s="8"/>
-      <c r="BC173" s="13"/>
-    </row>
-    <row r="174" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB174" s="8"/>
-      <c r="BC174" s="13"/>
-    </row>
-    <row r="175" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB175" s="8"/>
-      <c r="BC175" s="13"/>
-    </row>
-    <row r="176" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB176" s="8"/>
-      <c r="BC176" s="13"/>
-    </row>
-    <row r="177" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB177" s="8"/>
-      <c r="BC177" s="13"/>
-    </row>
-    <row r="178" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB178" s="8"/>
-      <c r="BC178" s="13"/>
-    </row>
-    <row r="179" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB179" s="8"/>
-      <c r="BC179" s="13"/>
-    </row>
-    <row r="180" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB180" s="8"/>
-      <c r="BC180" s="13"/>
-    </row>
-    <row r="181" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB181" s="8"/>
-      <c r="BC181" s="13"/>
-    </row>
-    <row r="182" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB182" s="8"/>
-      <c r="BC182" s="13"/>
-    </row>
-    <row r="183" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB183" s="8"/>
-      <c r="BC183" s="13"/>
-    </row>
-    <row r="184" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB184" s="8"/>
-      <c r="BC184" s="13"/>
-    </row>
-    <row r="185" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB185" s="8"/>
-      <c r="BC185" s="13"/>
-    </row>
-    <row r="186" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB186" s="8"/>
-      <c r="BC186" s="13"/>
-    </row>
-    <row r="187" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB187" s="8"/>
-      <c r="BC187" s="13"/>
-    </row>
-    <row r="188" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB188" s="8"/>
-      <c r="BC188" s="13"/>
-    </row>
-    <row r="189" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB189" s="8"/>
-      <c r="BC189" s="13"/>
-    </row>
-    <row r="190" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB190" s="8"/>
-      <c r="BC190" s="13"/>
-    </row>
-    <row r="191" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB191" s="8"/>
-      <c r="BC191" s="13"/>
-    </row>
-    <row r="192" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB192" s="8"/>
-      <c r="BC192" s="13"/>
-    </row>
-    <row r="193" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB193" s="8"/>
-      <c r="BC193" s="13"/>
-    </row>
-    <row r="194" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB194" s="8"/>
-      <c r="BC194" s="13"/>
-    </row>
-    <row r="195" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA168" s="8"/>
+      <c r="BB168" s="13"/>
+    </row>
+    <row r="169" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA169" s="8"/>
+      <c r="BB169" s="13"/>
+    </row>
+    <row r="170" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA170" s="8"/>
+      <c r="BB170" s="13"/>
+    </row>
+    <row r="171" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA171" s="8"/>
+      <c r="BB171" s="13"/>
+    </row>
+    <row r="172" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA172" s="8"/>
+      <c r="BB172" s="13"/>
+    </row>
+    <row r="173" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA173" s="8"/>
+      <c r="BB173" s="13"/>
+    </row>
+    <row r="174" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA174" s="8"/>
+      <c r="BB174" s="13"/>
+    </row>
+    <row r="175" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA175" s="8"/>
+      <c r="BB175" s="13"/>
+    </row>
+    <row r="176" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA176" s="8"/>
+      <c r="BB176" s="13"/>
+    </row>
+    <row r="177" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA177" s="8"/>
+      <c r="BB177" s="13"/>
+    </row>
+    <row r="178" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA178" s="8"/>
+      <c r="BB178" s="13"/>
+    </row>
+    <row r="179" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA179" s="8"/>
+      <c r="BB179" s="13"/>
+    </row>
+    <row r="180" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA180" s="8"/>
+      <c r="BB180" s="13"/>
+    </row>
+    <row r="181" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA181" s="8"/>
+      <c r="BB181" s="13"/>
+    </row>
+    <row r="182" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA182" s="8"/>
+      <c r="BB182" s="13"/>
+    </row>
+    <row r="183" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA183" s="8"/>
+      <c r="BB183" s="13"/>
+    </row>
+    <row r="184" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA184" s="8"/>
+      <c r="BB184" s="13"/>
+    </row>
+    <row r="185" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA185" s="8"/>
+      <c r="BB185" s="13"/>
+    </row>
+    <row r="186" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA186" s="8"/>
+      <c r="BB186" s="13"/>
+    </row>
+    <row r="187" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA187" s="8"/>
+      <c r="BB187" s="13"/>
+    </row>
+    <row r="188" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA188" s="8"/>
+      <c r="BB188" s="13"/>
+    </row>
+    <row r="189" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA189" s="8"/>
+      <c r="BB189" s="13"/>
+    </row>
+    <row r="190" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA190" s="8"/>
+      <c r="BB190" s="13"/>
+    </row>
+    <row r="191" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA191" s="8"/>
+      <c r="BB191" s="13"/>
+    </row>
+    <row r="192" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA192" s="8"/>
+      <c r="BB192" s="13"/>
+    </row>
+    <row r="193" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA193" s="8"/>
+      <c r="BB193" s="13"/>
+    </row>
+    <row r="194" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA194" s="8"/>
+      <c r="BB194" s="13"/>
+    </row>
+    <row r="195" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB195" s="16"/>
-      <c r="BB195" s="8"/>
-      <c r="BC195" s="13"/>
-    </row>
-    <row r="196" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB196" s="8"/>
-      <c r="BC196" s="13"/>
-    </row>
-    <row r="197" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB197" s="8"/>
-      <c r="BC197" s="13"/>
-    </row>
-    <row r="198" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA195" s="8"/>
+      <c r="BB195" s="13"/>
+    </row>
+    <row r="196" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA196" s="8"/>
+      <c r="BB196" s="13"/>
+    </row>
+    <row r="197" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA197" s="8"/>
+      <c r="BB197" s="13"/>
+    </row>
+    <row r="198" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB198" s="16"/>
-      <c r="BB198" s="8"/>
-      <c r="BC198" s="13"/>
-    </row>
-    <row r="199" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB199" s="8"/>
-      <c r="BC199" s="13"/>
-    </row>
-    <row r="200" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB200" s="8"/>
-      <c r="BC200" s="13"/>
-    </row>
-    <row r="201" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB201" s="8"/>
-      <c r="BC201" s="13"/>
-    </row>
-    <row r="202" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB202" s="8"/>
-      <c r="BC202" s="13"/>
-    </row>
-    <row r="203" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB203" s="8"/>
-      <c r="BC203" s="13"/>
-    </row>
-    <row r="204" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB204" s="8"/>
-      <c r="BC204" s="13"/>
-    </row>
-    <row r="205" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB205" s="8"/>
-      <c r="BC205" s="13"/>
-    </row>
-    <row r="206" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA198" s="8"/>
+      <c r="BB198" s="13"/>
+    </row>
+    <row r="199" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA199" s="8"/>
+      <c r="BB199" s="13"/>
+    </row>
+    <row r="200" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA200" s="8"/>
+      <c r="BB200" s="13"/>
+    </row>
+    <row r="201" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA201" s="8"/>
+      <c r="BB201" s="13"/>
+    </row>
+    <row r="202" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA202" s="8"/>
+      <c r="BB202" s="13"/>
+    </row>
+    <row r="203" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA203" s="8"/>
+      <c r="BB203" s="13"/>
+    </row>
+    <row r="204" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA204" s="8"/>
+      <c r="BB204" s="13"/>
+    </row>
+    <row r="205" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA205" s="8"/>
+      <c r="BB205" s="13"/>
+    </row>
+    <row r="206" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB206" s="11"/>
-      <c r="BB206" s="8"/>
-      <c r="BC206" s="13"/>
-    </row>
-    <row r="207" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB207" s="8"/>
-      <c r="BC207" s="13"/>
-    </row>
-    <row r="208" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB208" s="8"/>
-      <c r="BC208" s="13"/>
-    </row>
-    <row r="209" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB209" s="8"/>
-      <c r="BC209" s="13"/>
-    </row>
-    <row r="210" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB210" s="8"/>
-      <c r="BC210" s="13"/>
-    </row>
-    <row r="211" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB211" s="8"/>
-      <c r="BC211" s="13"/>
-    </row>
-    <row r="212" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB212" s="8"/>
-      <c r="BC212" s="13"/>
-    </row>
-    <row r="213" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB213" s="8"/>
-      <c r="BC213" s="13"/>
-    </row>
-    <row r="214" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB214" s="8"/>
-      <c r="BC214" s="13"/>
-    </row>
-    <row r="215" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB215" s="8"/>
-      <c r="BC215" s="13"/>
-    </row>
-    <row r="216" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA206" s="8"/>
+      <c r="BB206" s="13"/>
+    </row>
+    <row r="207" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA207" s="8"/>
+      <c r="BB207" s="13"/>
+    </row>
+    <row r="208" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA208" s="8"/>
+      <c r="BB208" s="13"/>
+    </row>
+    <row r="209" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA209" s="8"/>
+      <c r="BB209" s="13"/>
+    </row>
+    <row r="210" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA210" s="8"/>
+      <c r="BB210" s="13"/>
+    </row>
+    <row r="211" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA211" s="8"/>
+      <c r="BB211" s="13"/>
+    </row>
+    <row r="212" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA212" s="8"/>
+      <c r="BB212" s="13"/>
+    </row>
+    <row r="213" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA213" s="8"/>
+      <c r="BB213" s="13"/>
+    </row>
+    <row r="214" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA214" s="8"/>
+      <c r="BB214" s="13"/>
+    </row>
+    <row r="215" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA215" s="8"/>
+      <c r="BB215" s="13"/>
+    </row>
+    <row r="216" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB216" s="17"/>
-      <c r="BB216" s="8"/>
-      <c r="BC216" s="13"/>
-    </row>
-    <row r="217" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB217" s="8"/>
-      <c r="BC217" s="13"/>
-    </row>
-    <row r="218" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB218" s="8"/>
-      <c r="BC218" s="13"/>
-    </row>
-    <row r="219" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB219" s="8"/>
-      <c r="BC219" s="13"/>
-    </row>
-    <row r="220" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB220" s="8"/>
-      <c r="BC220" s="13"/>
-    </row>
-    <row r="221" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB221" s="8"/>
-      <c r="BC221" s="13"/>
-    </row>
-    <row r="222" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA216" s="8"/>
+      <c r="BB216" s="13"/>
+    </row>
+    <row r="217" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA217" s="8"/>
+      <c r="BB217" s="13"/>
+    </row>
+    <row r="218" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA218" s="8"/>
+      <c r="BB218" s="13"/>
+    </row>
+    <row r="219" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA219" s="8"/>
+      <c r="BB219" s="13"/>
+    </row>
+    <row r="220" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA220" s="8"/>
+      <c r="BB220" s="13"/>
+    </row>
+    <row r="221" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA221" s="8"/>
+      <c r="BB221" s="13"/>
+    </row>
+    <row r="222" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB222" s="15"/>
-      <c r="BB222" s="8"/>
-      <c r="BC222" s="13"/>
-    </row>
-    <row r="223" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB223" s="8"/>
-      <c r="BC223" s="13"/>
-    </row>
-    <row r="224" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB224" s="8"/>
-      <c r="BC224" s="13"/>
-    </row>
-    <row r="225" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA222" s="8"/>
+      <c r="BB222" s="13"/>
+    </row>
+    <row r="223" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA223" s="8"/>
+      <c r="BB223" s="13"/>
+    </row>
+    <row r="224" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA224" s="8"/>
+      <c r="BB224" s="13"/>
+    </row>
+    <row r="225" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB225" s="17"/>
-      <c r="BB225" s="8"/>
-      <c r="BC225" s="13"/>
-    </row>
-    <row r="226" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB226" s="8"/>
-      <c r="BC226" s="13"/>
-    </row>
-    <row r="227" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA225" s="8"/>
+      <c r="BB225" s="13"/>
+    </row>
+    <row r="226" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA226" s="8"/>
+      <c r="BB226" s="13"/>
+    </row>
+    <row r="227" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB227" s="11"/>
-      <c r="BB227" s="8"/>
-      <c r="BC227" s="13"/>
-    </row>
-    <row r="228" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB228" s="8"/>
-      <c r="BC228" s="13"/>
-    </row>
-    <row r="229" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB229" s="8"/>
-      <c r="BC229" s="13"/>
-    </row>
-    <row r="230" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB230" s="8"/>
-    </row>
-    <row r="231" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB231" s="8"/>
-      <c r="BC231" s="13"/>
-    </row>
-    <row r="232" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB232" s="8"/>
-      <c r="BC232" s="13"/>
-    </row>
-    <row r="233" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA227" s="8"/>
+      <c r="BB227" s="13"/>
+    </row>
+    <row r="228" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA228" s="8"/>
+      <c r="BB228" s="13"/>
+    </row>
+    <row r="229" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA229" s="8"/>
+      <c r="BB229" s="13"/>
+    </row>
+    <row r="230" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA230" s="8"/>
+    </row>
+    <row r="231" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA231" s="8"/>
+      <c r="BB231" s="13"/>
+    </row>
+    <row r="232" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA232" s="8"/>
+      <c r="BB232" s="13"/>
+    </row>
+    <row r="233" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB233" s="16"/>
-      <c r="BB233" s="8"/>
-      <c r="BC233" s="13"/>
-    </row>
-    <row r="234" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB234" s="8"/>
-      <c r="BC234" s="13"/>
-    </row>
-    <row r="235" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB235" s="8"/>
-      <c r="BC235" s="13"/>
-    </row>
-    <row r="236" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA233" s="8"/>
+      <c r="BB233" s="13"/>
+    </row>
+    <row r="234" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA234" s="8"/>
+      <c r="BB234" s="13"/>
+    </row>
+    <row r="235" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA235" s="8"/>
+      <c r="BB235" s="13"/>
+    </row>
+    <row r="236" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB236" s="16"/>
-      <c r="BB236" s="8"/>
-      <c r="BC236" s="13"/>
-    </row>
-    <row r="237" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB237" s="8"/>
-    </row>
-    <row r="238" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB238" s="8"/>
-      <c r="BC238" s="13"/>
-    </row>
-    <row r="239" spans="28:55" x14ac:dyDescent="0.35">
+      <c r="BA236" s="8"/>
+      <c r="BB236" s="13"/>
+    </row>
+    <row r="237" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA237" s="8"/>
+    </row>
+    <row r="238" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA238" s="8"/>
+      <c r="BB238" s="13"/>
+    </row>
+    <row r="239" spans="28:54" x14ac:dyDescent="0.35">
       <c r="AB239" s="11"/>
-      <c r="BB239" s="8"/>
-      <c r="BC239" s="13"/>
-    </row>
-    <row r="240" spans="28:55" x14ac:dyDescent="0.35">
-      <c r="BB240" s="8"/>
-      <c r="BC240" s="13"/>
-    </row>
-    <row r="241" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB241" s="8"/>
-      <c r="BC241" s="13"/>
-    </row>
-    <row r="242" spans="54:55" x14ac:dyDescent="0.35">
-      <c r="BB242" s="8"/>
-      <c r="BC242" s="13"/>
+      <c r="BA239" s="8"/>
+      <c r="BB239" s="13"/>
+    </row>
+    <row r="240" spans="28:54" x14ac:dyDescent="0.35">
+      <c r="BA240" s="8"/>
+      <c r="BB240" s="13"/>
+    </row>
+    <row r="241" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA241" s="8"/>
+      <c r="BB241" s="13"/>
+    </row>
+    <row r="242" spans="53:54" x14ac:dyDescent="0.35">
+      <c r="BA242" s="8"/>
+      <c r="BB242" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="19">
@@ -6958,7 +6970,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AF1048576">
       <formula1>City</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2:AT1048576 AG2:AG1048576 AW2:AX1048576 BA2:BA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2:AT1048576 AG2:AG1048576 AW2:AW1048576 AZ2:AZ1048576">
       <formula1>Yes_No</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2:AV1048576">
@@ -6992,7 +7004,7 @@
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2:AX1048576">
       <formula1>Ported</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2:AS1048576">
@@ -7001,15 +7013,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2:AR11 AR13:AR99 AR101:AR133 AR135:AR236 AR243:AR1048576 AR238:AR241">
       <formula1>Handset</formula1>
     </dataValidation>
-    <dataValidation type="date" showInputMessage="1" showErrorMessage="1" sqref="BB2:BB1048576">
+    <dataValidation type="date" showInputMessage="1" showErrorMessage="1" sqref="BA2:BA1048576">
       <formula1>43476</formula1>
       <formula2>47484</formula2>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC2:BC1048576">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2:BB1048576">
       <formula1>0.375</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2:BD1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC2:BC1048576">
       <formula1>Mode_Meeting</formula1>
     </dataValidation>
   </dataValidations>
@@ -7020,7 +7032,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$AE$2:$AE$16</xm:f>
+            <xm:f>Lists!$AE$2:$AE$18</xm:f>
           </x14:formula1>
           <xm:sqref>AB2:AB1048576</xm:sqref>
         </x14:dataValidation>
@@ -7034,8 +7046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE10953"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+    <sheetView topLeftCell="P2" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2:AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7603,7 +7615,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>78</v>
       </c>
@@ -7616,8 +7628,11 @@
       <c r="I17">
         <v>2111005</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="AE17" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>79</v>
       </c>
@@ -7630,8 +7645,11 @@
       <c r="I18">
         <v>3111005</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="AE18" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>80</v>
       </c>
@@ -7645,7 +7663,7 @@
         <v>1111005</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>81</v>
       </c>
@@ -7659,7 +7677,7 @@
         <v>1111006</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>82</v>
       </c>
@@ -7673,7 +7691,7 @@
         <v>2111006</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>83</v>
       </c>
@@ -7687,7 +7705,7 @@
         <v>3111006</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>84</v>
       </c>
@@ -7701,7 +7719,7 @@
         <v>1111007</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>85</v>
       </c>
@@ -7715,7 +7733,7 @@
         <v>2111007</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>86</v>
       </c>
@@ -7729,7 +7747,7 @@
         <v>3111007</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>87</v>
       </c>
@@ -7743,7 +7761,7 @@
         <v>2111008</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>88</v>
       </c>
@@ -7757,7 +7775,7 @@
         <v>3111008</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>89</v>
       </c>
@@ -7771,7 +7789,7 @@
         <v>1111008</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>90</v>
       </c>
@@ -7785,7 +7803,7 @@
         <v>3111009</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>91</v>
       </c>
@@ -7799,7 +7817,7 @@
         <v>1111009</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>92</v>
       </c>
@@ -7813,7 +7831,7 @@
         <v>2111009</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:31" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>93</v>
       </c>

</xml_diff>